<commit_message>
atualizacao dos dados para o dash
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Dia</t>
   </si>
@@ -43,10 +43,19 @@
     <t>2025-03-18</t>
   </si>
   <si>
+    <t>2025-03-21</t>
+  </si>
+  <si>
+    <t>CARBOMAN-GAS CARBONICO DE MANAUS LTDA</t>
+  </si>
+  <si>
+    <t>59.609.849 LEANDRO CARVALHO DA SILVA</t>
+  </si>
+  <si>
     <t>MUSASHI DA AMAZONIA LTDA</t>
   </si>
   <si>
-    <t>CARBOMAN-GAS CARBONICO DE MANAUS LTDA</t>
+    <t>GERBERA COSMETICOS LTDA</t>
   </si>
   <si>
     <t>V V REFEICOES LTDA</t>
@@ -55,61 +64,145 @@
     <t>METALURGICA SATO DA AMAZONIA LTDA</t>
   </si>
   <si>
-    <t>GERBERA COSMETICOS LTDA</t>
+    <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+  </si>
+  <si>
+    <t>000098</t>
+  </si>
+  <si>
+    <t>000439</t>
+  </si>
+  <si>
+    <t>000052</t>
+  </si>
+  <si>
+    <t>000568</t>
   </si>
   <si>
     <t>000415</t>
   </si>
   <si>
-    <t>000568</t>
+    <t>000053</t>
+  </si>
+  <si>
+    <t>000914</t>
+  </si>
+  <si>
+    <t>000307</t>
+  </si>
+  <si>
+    <t>010456</t>
+  </si>
+  <si>
+    <t>000839</t>
+  </si>
+  <si>
+    <t>010302</t>
+  </si>
+  <si>
+    <t>000660</t>
+  </si>
+  <si>
+    <t>010178</t>
   </si>
   <si>
     <t>000243</t>
   </si>
   <si>
+    <t>010072</t>
+  </si>
+  <si>
+    <t>010027</t>
+  </si>
+  <si>
+    <t>000579</t>
+  </si>
+  <si>
+    <t>010633</t>
+  </si>
+  <si>
+    <t>000548</t>
+  </si>
+  <si>
     <t>000219</t>
   </si>
   <si>
-    <t>010072</t>
-  </si>
-  <si>
     <t>010002</t>
   </si>
   <si>
-    <t>000548</t>
-  </si>
-  <si>
-    <t>000660</t>
-  </si>
-  <si>
-    <t>000839</t>
+    <t>000004</t>
+  </si>
+  <si>
+    <t>000122</t>
+  </si>
+  <si>
+    <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
+  </si>
+  <si>
+    <t>LUVA DE LIMPEZA LATEX TAM P VERDE NOBRE CA 41506</t>
+  </si>
+  <si>
+    <t>PAPEL ALUMINIO 30CMx100M</t>
+  </si>
+  <si>
+    <t>LIMPA ALUMINIO 5L GLOBO SAN</t>
   </si>
   <si>
     <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
   </si>
   <si>
-    <t>LIMPA ALUMINIO 5L GLOBO SAN</t>
+    <t>FILME PVC 28X300M ALPFILM</t>
+  </si>
+  <si>
+    <t>LUVA DE LIMPEZA LATEX TAM G VERDE NOBRE SLIM CA 41506</t>
+  </si>
+  <si>
+    <t>DISCO REMOVEDOR PRETO P ENCERADEIRA 510MM</t>
+  </si>
+  <si>
+    <t>CLIPS 4/0 C/50 UNDS NIQUELADO CHAPARRAU</t>
+  </si>
+  <si>
+    <t>ACUCAR CRISTAL ITAMARATI 1KG</t>
+  </si>
+  <si>
+    <t>CAFE TORRADO E MOIDO CLASSICO ALMOFADA SANTA CLARA 250G</t>
+  </si>
+  <si>
+    <t>PAPEL HIGIENICO FLORAL PERFUMADO C/4 ROLOS</t>
+  </si>
+  <si>
+    <t>MARCA TEXTO AMARELO UND JOCAR OFFICE</t>
   </si>
   <si>
     <t>FIBRA DE LIMPEZA PESADA 102X260mm</t>
   </si>
   <si>
+    <t>FITA DUREX 48 X 50 TRANSPARENTE</t>
+  </si>
+  <si>
+    <t>REGUA PLASTICA 30 CM LEO E LEO</t>
+  </si>
+  <si>
+    <t>LIVRO PROTOCOLO DE CORRESPONDENCIA 104 FLS</t>
+  </si>
+  <si>
+    <t>CANETA CRISTAL MEDIA AZUL BIC</t>
+  </si>
+  <si>
+    <t>BOBINA TERMICA 80X40 BRANCA 1VIA RIO BRANCO</t>
+  </si>
+  <si>
     <t>FIBRA DE LIMPEZA USO GERAL 102X260mm</t>
   </si>
   <si>
-    <t>FITA DUREX 48 X 50 TRANSPARENTE</t>
-  </si>
-  <si>
     <t>PINCEL ATOMICO PILOT 1100P PRETO</t>
   </si>
   <si>
-    <t>BOBINA TERMICA 80X40 BRANCA 1VIA RIO BRANCO</t>
-  </si>
-  <si>
-    <t>PAPEL HIGIENICO FLORAL PERFUMADO C/4 ROLOS</t>
-  </si>
-  <si>
-    <t>ACUCAR CRISTAL ITAMARATI 1KG</t>
+    <t>ALCOOL LIQUIDO FACILITA 70% INPM 5L</t>
+  </si>
+  <si>
+    <t>SABAO EM PO ALA LAVANDA ROUPAS 400G</t>
   </si>
 </sst>
 </file>
@@ -467,7 +560,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -498,77 +591,77 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2">
-        <v>90</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="G2">
-        <v>4</v>
+        <v>972</v>
       </c>
       <c r="H2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G3">
-        <v>33</v>
+        <v>133</v>
       </c>
       <c r="H3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>300</v>
+        <v>120</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="G4">
-        <v>702</v>
+        <v>2</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -576,25 +669,25 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>300</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="G5">
-        <v>1278</v>
+        <v>33</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -602,103 +695,103 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="G6">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="H6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8">
-        <v>450</v>
+        <v>160</v>
       </c>
       <c r="D8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="G8">
-        <v>26</v>
+        <v>426</v>
       </c>
       <c r="H8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
       <c r="C9">
-        <v>320</v>
+        <v>60</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="G9">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -706,27 +799,391 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10">
-        <v>256</v>
+        <v>30</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>26</v>
+      </c>
+      <c r="H10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>512</v>
+      </c>
+      <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>13</v>
+      </c>
+      <c r="H11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>260</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>640</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13">
+        <v>186</v>
+      </c>
+      <c r="H13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
+        <v>120</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14">
+        <v>70</v>
+      </c>
+      <c r="H14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15">
+        <v>600</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15">
+        <v>701</v>
+      </c>
+      <c r="H15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16">
+        <v>400</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" t="s">
         <v>31</v>
       </c>
-      <c r="G10">
-        <v>28</v>
-      </c>
-      <c r="H10" t="b">
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16">
+        <v>43</v>
+      </c>
+      <c r="H16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17">
+        <v>70</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="1">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F18" t="s">
+        <v>56</v>
+      </c>
+      <c r="G18">
+        <v>-4</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="1">
+        <v>21</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19">
+        <v>2300</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19">
+        <v>148</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="1">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20">
+        <v>900</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20">
+        <v>26</v>
+      </c>
+      <c r="H20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21">
+        <v>600</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" t="s">
+        <v>59</v>
+      </c>
+      <c r="G21">
+        <v>1268</v>
+      </c>
+      <c r="H21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="1">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22">
+        <v>144</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>60</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="1">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23" t="s">
+        <v>61</v>
+      </c>
+      <c r="G23">
+        <v>89</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="1">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>200</v>
+      </c>
+      <c r="D24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24">
+        <v>268</v>
+      </c>
+      <c r="H24" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
coloquei na main as alterações da giovanna
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Dia</t>
   </si>
@@ -37,52 +37,40 @@
     <t>critico</t>
   </si>
   <si>
-    <t>2025-03-21</t>
+    <t>2025-03-19</t>
   </si>
   <si>
     <t>2025-03-24</t>
   </si>
   <si>
+    <t>ZARAPLAST DA AMAZONIA LTDA</t>
+  </si>
+  <si>
     <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
   </si>
   <si>
-    <t>REVEMAR COMERCIO DE MOTOS LTDA</t>
-  </si>
-  <si>
-    <t>J R BASTOS</t>
-  </si>
-  <si>
-    <t>LUCAS CLIENTE NOVO</t>
-  </si>
-  <si>
-    <t>000122</t>
-  </si>
-  <si>
-    <t>000434</t>
-  </si>
-  <si>
-    <t>000349</t>
-  </si>
-  <si>
-    <t>000158</t>
-  </si>
-  <si>
-    <t>010456</t>
-  </si>
-  <si>
-    <t>SABAO EM PO ALA LAVANDA ROUPAS 400G</t>
-  </si>
-  <si>
-    <t>FRASCO COM VALVULA PUMP 450ML (p/alcool/sabonete) - NOBRE</t>
-  </si>
-  <si>
-    <t>DESODORISADOR LADY AEROSSOL 360ML TALCO SUAVE CARINHO</t>
-  </si>
-  <si>
-    <t>AZULIM LIMPA CERAMICAS E AZULEJOS LAVANDA 5L 1:15 START</t>
-  </si>
-  <si>
-    <t>CLIPS 4/0 C/50 UNDS NIQUELADO CHAPARRAU</t>
+    <t>000098</t>
+  </si>
+  <si>
+    <t>000276</t>
+  </si>
+  <si>
+    <t>000146</t>
+  </si>
+  <si>
+    <t>000088</t>
+  </si>
+  <si>
+    <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
+  </si>
+  <si>
+    <t>INSETICIDA SBP AEROSSOL 380ML</t>
+  </si>
+  <si>
+    <t>DESINFETANTE BRINORT 2L LAVANDA</t>
+  </si>
+  <si>
+    <t>VASSOURA PIACAVA 20 FUROS</t>
   </si>
 </sst>
 </file>
@@ -440,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -471,7 +459,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -483,13 +471,13 @@
         <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2">
-        <v>258</v>
+        <v>939</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -497,105 +485,79 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G3">
-        <v>65</v>
+        <v>-2</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>1248</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G4">
-        <v>1225</v>
+        <v>13</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="G5">
-        <v>60</v>
+        <v>-50</v>
       </c>
       <c r="H5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6">
-        <v>70</v>
-      </c>
-      <c r="D6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6">
-        <v>24</v>
-      </c>
-      <c r="H6" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add updates to vendas_atipicas_atual.xlsx
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,33 +472,33 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-03-12</t>
+          <t>2025-03-13</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>200</v>
+        <v>360</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+          <t>AMMAC INDUSTRIA E COMERCIO DE ALIMENTOS LTDA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>000779</t>
+          <t>000029</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PEDRA SANITARIA NAFT PLUS FLORAL 25G</t>
+          <t>ESPONJA MULTIUSO JEITOSA</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>-68</v>
+        <v>2416</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -506,67 +506,67 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2025-03-13</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>50</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>E A H EMPRESA AMAZONENSE DE HOTELARIA LTDA</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>000440</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>LUVA DE LIMPEZA LATEX TAM M AMARELA TOP REFOR NOBRE CA 47259</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>292</v>
+      </c>
+      <c r="H3" t="b">
         <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2025-03-12</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>200</v>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MUSASHI DA AMAZONIA LTDA</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>000098</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>429</v>
-      </c>
-      <c r="H3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-03-13</t>
+          <t>2025-03-14</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>360</v>
+        <v>27</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>AMMAC INDUSTRIA E COMERCIO DE ALIMENTOS LTDA</t>
+          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>000029</t>
+          <t>000152</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ESPONJA MULTIUSO JEITOSA</t>
+          <t>COPO DESCARTAVEL BRANCO CRISTALCOPO 180ML CX C\25</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>2419</v>
+        <v>56</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -582,7 +582,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -591,16 +591,16 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>000152</t>
+          <t>000924</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>COPO DESCARTAVEL BRANCO CRISTALCOPO 180ML CX C\25</t>
+          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -608,41 +608,41 @@
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2025-03-14</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+          <t>MUSASHI DA AMAZONIA LTDA</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>000924</t>
+          <t>000415</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
+          <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
         </is>
       </c>
       <c r="G6" t="n">
+        <v>3</v>
+      </c>
+      <c r="H6" t="b">
         <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -668,7 +668,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>379</v>
+        <v>351</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -684,33 +684,33 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>180</v>
+        <v>40</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>MUSASHI DA AMAZONIA LTDA</t>
+          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>000415</t>
+          <t>000078</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
+          <t>SACO DE LIXO 100L PRETO COMUM - PCT C/100 UND</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="H8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -718,7 +718,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -727,16 +727,16 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>000842</t>
+          <t>000243</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 200L COMUM PACOTINHO C/5 UND</t>
+          <t>FIBRA DE LIMPEZA PESADA 102X260mm</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>426</v>
+        <v>661</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -761,16 +761,16 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>000078</t>
+          <t>000071</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 100L PRETO COMUM - PCT C/100 UND</t>
+          <t>SACO DE LIXO 200L PRETO COMUM - PCT C/100 UND</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -778,7 +778,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -786,25 +786,25 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>36</v>
+        <v>400</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
+          <t>MUSASHI DA AMAZONIA LTDA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>000071</t>
+          <t>000842</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 200L PRETO COMUM - PCT C/100 UND</t>
+          <t>SACO DE LIXO 200L COMUM PACOTINHO C/5 UND</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>17</v>
+        <v>426</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -812,33 +812,33 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>MUSASHI DA AMAZONIA LTDA</t>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>000243</t>
+          <t>000276</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>FIBRA DE LIMPEZA PESADA 102X260mm</t>
+          <t>INSETICIDA SBP AEROSSOL 380ML</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>681</v>
+        <v>50</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -846,7 +846,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -863,16 +863,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>000276</t>
+          <t>000146</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>INSETICIDA SBP AEROSSOL 380ML</t>
+          <t>DESINFETANTE BRINORT 2L LAVANDA</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -880,7 +880,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -888,25 +888,25 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>200</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+          <t>ZARAPLAST DA AMAZONIA LTDA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>000146</t>
+          <t>000098</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>DESINFETANTE BRINORT 2L LAVANDA</t>
+          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>13</v>
+        <v>311</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -914,33 +914,33 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>2025-03-24</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>150</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>000088</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>VASSOURA PIACAVA 20 FUROS</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>2</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>2025-03-19</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>200</v>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>ZARAPLAST DA AMAZONIA LTDA</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>000098</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>429</v>
       </c>
       <c r="H15" t="b">
         <v>0</v>
@@ -948,33 +948,33 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>000088</t>
+          <t>000288</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>VASSOURA PIACAVA 20 FUROS</t>
+          <t>TOUCA DESCARTAVEL TNT TALGE PCT C/ 100 UND</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>-52</v>
+        <v>400</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -990,33 +990,33 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>120</v>
+        <v>15</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>000350</t>
+          <t>000924</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
+          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>960</v>
+        <v>1</v>
       </c>
       <c r="H17" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1024,33 +1024,33 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>96</v>
+        <v>120</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
+          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>000032</t>
+          <t>000350</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
+          <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1386</v>
+        <v>1017</v>
       </c>
       <c r="H18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1058,25 +1058,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>300</v>
+        <v>96</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>000098</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
+          <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>429</v>
+        <v>1382</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1101,16 +1101,16 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>000486</t>
+          <t>000098</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>NAFTALINA 40G PCT RUBI</t>
+          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1126,25 +1126,25 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MANJAR SERVICOS GERAIS SA</t>
+          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>000583</t>
+          <t>000486</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>LIMPA ALUMINIO BRINORT 500ML</t>
+          <t>NAFTALINA 40G PCT RUBI</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>221</v>
+        <v>310</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1152,7 +1152,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1160,25 +1160,25 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
+          <t>MANJAR SERVICOS GERAIS SA</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>000288</t>
+          <t>000583</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>TOUCA DESCARTAVEL TNT TALGE PCT C/ 100 UND</t>
+          <t>LIMPA ALUMINIO BRINORT 500ML</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>415</v>
+        <v>221</v>
       </c>
       <c r="H22" t="b">
         <v>0</v>
@@ -1186,35 +1186,69 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>2025-03-26</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
         <v>10</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2025-03-25</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>15</v>
-      </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>000924</t>
+          <t>000425</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
+          <t>COADOR DE CAFE EG (EXTRA GRANDE)</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>2025-03-26</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>200</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>000122</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>SABAO EM PO ALA LAVANDA ROUPAS 400G</t>
+        </is>
+      </c>
+      <c r="G24" t="n">
+        <v>58</v>
+      </c>
+      <c r="H24" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated relatorio_produtos and vendas_atipicas_atual files
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,33 +472,33 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2025-03-13</t>
+          <t>2025-03-14</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>360</v>
+        <v>27</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>AMMAC INDUSTRIA E COMERCIO DE ALIMENTOS LTDA</t>
+          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>000029</t>
+          <t>000152</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ESPONJA MULTIUSO JEITOSA</t>
+          <t>COPO DESCARTAVEL BRANCO CRISTALCOPO 180ML CX C\25</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>2416</v>
+        <v>45</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -506,67 +506,67 @@
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>2025-03-13</t>
+          <t>2025-03-14</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>E A H EMPRESA AMAZONENSE DE HOTELARIA LTDA</t>
+          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>000440</t>
+          <t>000924</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>LUVA DE LIMPEZA LATEX TAM M AMARELA TOP REFOR NOBRE CA 47259</t>
+          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>292</v>
+        <v>57</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2025-03-14</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>000152</t>
+          <t>000078</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>COPO DESCARTAVEL BRANCO CRISTALCOPO 180ML CX C\25</t>
+          <t>SACO DE LIXO 100L PRETO COMUM - PCT C/100 UND</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -574,41 +574,41 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2025-03-14</t>
+          <t>2025-03-17</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>11</v>
+        <v>180</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+          <t>MUSASHI DA AMAZONIA LTDA</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>000924</t>
+          <t>000415</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
+          <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
         </is>
       </c>
       <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="b">
         <v>1</v>
-      </c>
-      <c r="H5" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>180</v>
+        <v>400</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -625,24 +625,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>000415</t>
+          <t>000842</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
+          <t>SACO DE LIXO 200L COMUM PACOTINHO C/5 UND</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>3</v>
+        <v>416</v>
       </c>
       <c r="H6" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -650,25 +650,25 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>432</v>
+        <v>36</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>DSB COMERCIO DE ALIMENTOS EIRELI</t>
+          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>000717</t>
+          <t>000071</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>DETERGENTE NEUTRO BRINORT 500ML</t>
+          <t>SACO DE LIXO 200L PRETO COMUM - PCT C/100 UND</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>351</v>
+        <v>7</v>
       </c>
       <c r="H7" t="b">
         <v>0</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -684,25 +684,25 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>40</v>
+        <v>432</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
+          <t>DSB COMERCIO DE ALIMENTOS EIRELI</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>000078</t>
+          <t>000717</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 100L PRETO COMUM - PCT C/100 UND</t>
+          <t>DETERGENTE NEUTRO BRINORT 500ML</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>72</v>
+        <v>328</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -744,33 +744,33 @@
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>000071</t>
+          <t>000276</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 200L PRETO COMUM - PCT C/100 UND</t>
+          <t>INSETICIDA SBP AEROSSOL 380ML</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -778,33 +778,33 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>2025-03-17</t>
+          <t>2025-03-19</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>MUSASHI DA AMAZONIA LTDA</t>
+          <t>ZARAPLAST DA AMAZONIA LTDA</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>000842</t>
+          <t>000098</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>SACO DE LIXO 200L COMUM PACOTINHO C/5 UND</t>
+          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>426</v>
+        <v>287</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -829,16 +829,16 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>000276</t>
+          <t>000146</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>INSETICIDA SBP AEROSSOL 380ML</t>
+          <t>DESINFETANTE BRINORT 2L LAVANDA</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -846,15 +846,15 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-24</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>150</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -863,16 +863,16 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>000146</t>
+          <t>000088</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>DESINFETANTE BRINORT 2L LAVANDA</t>
+          <t>VASSOURA PIACAVA 20 FUROS</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>42</v>
+        <v>2</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -880,33 +880,33 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2025-03-19</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>ZARAPLAST DA AMAZONIA LTDA</t>
+          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>000098</t>
+          <t>000288</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
+          <t>TOUCA DESCARTAVEL TNT TALGE PCT C/ 100 UND</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>311</v>
+        <v>399</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -914,41 +914,41 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>2025-03-24</t>
+          <t>2025-03-25</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>150</v>
+        <v>120</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
+          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>000088</t>
+          <t>000350</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>VASSOURA PIACAVA 20 FUROS</t>
+          <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>2</v>
+        <v>1005</v>
       </c>
       <c r="H15" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -956,25 +956,25 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
+          <t>MANJAR SERVICOS GERAIS SA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>000288</t>
+          <t>000583</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>TOUCA DESCARTAVEL TNT TALGE PCT C/ 100 UND</t>
+          <t>LIMPA ALUMINIO BRINORT 500ML</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>400</v>
+        <v>209</v>
       </c>
       <c r="H16" t="b">
         <v>0</v>
@@ -982,7 +982,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -990,25 +990,25 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>15</v>
+        <v>96</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>000924</t>
+          <t>000032</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
+          <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>1</v>
+        <v>1344</v>
       </c>
       <c r="H17" t="b">
         <v>0</v>
@@ -1016,7 +1016,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1024,7 +1024,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>120</v>
+        <v>300</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1033,24 +1033,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>000350</t>
+          <t>000098</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
+          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1017</v>
+        <v>287</v>
       </c>
       <c r="H18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1058,25 +1058,25 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
+          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>000032</t>
+          <t>000486</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
+          <t>NAFTALINA 40G PCT RUBI</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>1382</v>
+        <v>304</v>
       </c>
       <c r="H19" t="b">
         <v>0</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1092,25 +1092,25 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>300</v>
+        <v>15</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+          <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>000098</t>
+          <t>000924</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
+          <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>311</v>
+        <v>57</v>
       </c>
       <c r="H20" t="b">
         <v>0</v>
@@ -1118,33 +1118,33 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>000486</t>
+          <t>000425</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>NAFTALINA 40G PCT RUBI</t>
+          <t>COADOR DE CAFE EG (EXTRA GRANDE)</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>310</v>
+        <v>5</v>
       </c>
       <c r="H21" t="b">
         <v>0</v>
@@ -1152,103 +1152,35 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>2025-03-25</t>
+          <t>2025-03-26</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>96</v>
+        <v>200</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>MANJAR SERVICOS GERAIS SA</t>
+          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>000583</t>
+          <t>000122</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>LIMPA ALUMINIO BRINORT 500ML</t>
+          <t>SABAO EM PO ALA LAVANDA ROUPAS 400G</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>221</v>
+        <v>56</v>
       </c>
       <c r="H22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="1" t="n">
-        <v>8</v>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>2025-03-26</t>
-        </is>
-      </c>
-      <c r="C23" t="n">
-        <v>10</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>000425</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>COADOR DE CAFE EG (EXTRA GRANDE)</t>
-        </is>
-      </c>
-      <c r="G23" t="n">
-        <v>5</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="1" t="n">
-        <v>14</v>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>2025-03-26</t>
-        </is>
-      </c>
-      <c r="C24" t="n">
-        <v>200</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>000122</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>SABAO EM PO ALA LAVANDA ROUPAS 400G</t>
-        </is>
-      </c>
-      <c r="G24" t="n">
-        <v>58</v>
-      </c>
-      <c r="H24" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update arquivos .xlsx de recomendacao_compra e vendas_atipicas
</commit_message>
<xml_diff>
--- a/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
+++ b/dados/ADD/Dados_ADD_PF/vendas_atipicas_atual.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>Dia</t>
   </si>
@@ -37,9 +37,6 @@
     <t>critico</t>
   </si>
   <si>
-    <t>2025-03-17</t>
-  </si>
-  <si>
     <t>2025-03-19</t>
   </si>
   <si>
@@ -55,54 +52,27 @@
     <t>2025-03-28</t>
   </si>
   <si>
-    <t>POTENCIAL HUMANO RECRUTAMENTO E SELECAO LTDA</t>
-  </si>
-  <si>
-    <t>MUSASHI DA AMAZONIA LTDA</t>
-  </si>
-  <si>
-    <t>DSB COMERCIO DE ALIMENTOS EIRELI</t>
-  </si>
-  <si>
     <t>ZARAPLAST DA AMAZONIA LTDA</t>
   </si>
   <si>
     <t>JURUA ESTALEIROS E NAVEGACAO LTDA</t>
   </si>
   <si>
+    <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
+  </si>
+  <si>
     <t>MM DA AMAZONIA INDUSTRIA E COMERCIO DE PLASTICOS LTDA.</t>
   </si>
   <si>
+    <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
+  </si>
+  <si>
     <t>MANJAR SERVICOS GERAIS SA</t>
   </si>
   <si>
-    <t>MAP SERVICOS DE CONSERVACAO - EIRELI</t>
-  </si>
-  <si>
-    <t>AMAZONIA REFEICOES E SERVICOS LTDA</t>
-  </si>
-  <si>
     <t>AMAZONPEL COMERCIO DE MATERIAIS DE LIMPEZA LTDA</t>
   </si>
   <si>
-    <t>000078</t>
-  </si>
-  <si>
-    <t>000415</t>
-  </si>
-  <si>
-    <t>000842</t>
-  </si>
-  <si>
-    <t>000071</t>
-  </si>
-  <si>
-    <t>000717</t>
-  </si>
-  <si>
-    <t>000243</t>
-  </si>
-  <si>
     <t>000098</t>
   </si>
   <si>
@@ -115,24 +85,24 @@
     <t>000088</t>
   </si>
   <si>
+    <t>000350</t>
+  </si>
+  <si>
     <t>000288</t>
   </si>
   <si>
+    <t>000924</t>
+  </si>
+  <si>
+    <t>000032</t>
+  </si>
+  <si>
+    <t>000486</t>
+  </si>
+  <si>
     <t>000583</t>
   </si>
   <si>
-    <t>000032</t>
-  </si>
-  <si>
-    <t>000486</t>
-  </si>
-  <si>
-    <t>000350</t>
-  </si>
-  <si>
-    <t>000924</t>
-  </si>
-  <si>
     <t>000425</t>
   </si>
   <si>
@@ -142,24 +112,6 @@
     <t>000494</t>
   </si>
   <si>
-    <t>SACO DE LIXO 100L PRETO COMUM - PCT C/100 UND</t>
-  </si>
-  <si>
-    <t>DETERGENTE DESENGRAX MAX PINE AUDAX 5L</t>
-  </si>
-  <si>
-    <t>SACO DE LIXO 200L COMUM PACOTINHO C/5 UND</t>
-  </si>
-  <si>
-    <t>SACO DE LIXO 200L PRETO COMUM - PCT C/100 UND</t>
-  </si>
-  <si>
-    <t>DETERGENTE NEUTRO BRINORT 500ML</t>
-  </si>
-  <si>
-    <t>FIBRA DE LIMPEZA PESADA 102X260mm</t>
-  </si>
-  <si>
     <t>PANO DE CHAO FLANELADO C REFORCADO ITATEX 42x62CM</t>
   </si>
   <si>
@@ -172,22 +124,22 @@
     <t>VASSOURA PIACAVA 20 FUROS</t>
   </si>
   <si>
+    <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
+  </si>
+  <si>
     <t>TOUCA DESCARTAVEL TNT TALGE PCT C/ 100 UND</t>
   </si>
   <si>
+    <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
+  </si>
+  <si>
+    <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
+  </si>
+  <si>
+    <t>NAFTALINA 40G PCT RUBI</t>
+  </si>
+  <si>
     <t>LIMPA ALUMINIO BRINORT 500ML</t>
-  </si>
-  <si>
-    <t>LIMPADOR VEJA MULTIUSO GOLD 500ML</t>
-  </si>
-  <si>
-    <t>NAFTALINA 40G PCT RUBI</t>
-  </si>
-  <si>
-    <t>DESODORISADOR LADY AEROSSOL 360 ML LAVANDA</t>
-  </si>
-  <si>
-    <t>COPO POTE DESCARTAVEL TRANSP 100ML CX/20</t>
   </si>
   <si>
     <t>COADOR DE CAFE EG (EXTRA GRANDE)</t>
@@ -554,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -591,19 +543,19 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>40</v>
+        <v>200</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2">
         <v>23</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2">
-        <v>68</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -611,51 +563,51 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
-        <v>180</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="H3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>400</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="G4">
-        <v>416</v>
+        <v>8</v>
       </c>
       <c r="H4" t="b">
         <v>0</v>
@@ -663,25 +615,25 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5">
-        <v>36</v>
+        <v>150</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>229</v>
       </c>
       <c r="H5" t="b">
         <v>0</v>
@@ -689,25 +641,25 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>300</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>432</v>
-      </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="G6">
-        <v>280</v>
+        <v>23</v>
       </c>
       <c r="H6" t="b">
         <v>0</v>
@@ -715,51 +667,51 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
         <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G7">
-        <v>659</v>
+        <v>979</v>
       </c>
       <c r="H7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C8">
-        <v>200</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="G8">
-        <v>253</v>
+        <v>399</v>
       </c>
       <c r="H8" t="b">
         <v>0</v>
@@ -767,25 +719,25 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>30</v>
-      </c>
       <c r="F9" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="G9">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="H9" t="b">
         <v>0</v>
@@ -793,25 +745,25 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10">
-        <v>30</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="G10">
-        <v>8</v>
+        <v>1324</v>
       </c>
       <c r="H10" t="b">
         <v>0</v>
@@ -819,25 +771,25 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11">
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="F11" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="G11">
-        <v>-4</v>
+        <v>298</v>
       </c>
       <c r="H11" t="b">
         <v>0</v>
@@ -845,25 +797,25 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="G12">
-        <v>399</v>
+        <v>185</v>
       </c>
       <c r="H12" t="b">
         <v>0</v>
@@ -871,25 +823,25 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13">
-        <v>96</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G13">
-        <v>209</v>
+        <v>5</v>
       </c>
       <c r="H13" t="b">
         <v>0</v>
@@ -897,25 +849,25 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="G14">
-        <v>253</v>
+        <v>-3</v>
       </c>
       <c r="H14" t="b">
         <v>0</v>
@@ -923,183 +875,27 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="1">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
       <c r="C15">
-        <v>96</v>
+        <v>350</v>
       </c>
       <c r="D15" t="s">
         <v>18</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="G15">
-        <v>1331</v>
+        <v>438</v>
       </c>
       <c r="H15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="1">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>200</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
-        <v>36</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16">
-        <v>304</v>
-      </c>
-      <c r="H16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="1">
-        <v>4</v>
-      </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17">
-        <v>120</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17">
-        <v>1005</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="1">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>57</v>
-      </c>
-      <c r="G18">
-        <v>57</v>
-      </c>
-      <c r="H18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="1">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19">
-        <v>10</v>
-      </c>
-      <c r="D19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" t="s">
-        <v>58</v>
-      </c>
-      <c r="G19">
-        <v>5</v>
-      </c>
-      <c r="H19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="1">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20">
-        <v>200</v>
-      </c>
-      <c r="D20" t="s">
-        <v>17</v>
-      </c>
-      <c r="E20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" t="s">
-        <v>59</v>
-      </c>
-      <c r="G20">
-        <v>36</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="1">
-        <v>15</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21">
-        <v>350</v>
-      </c>
-      <c r="D21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21">
-        <v>438</v>
-      </c>
-      <c r="H21" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>